<commit_message>
Minor flow cleanup and commenting
</commit_message>
<xml_diff>
--- a/RHNA/output/rhna_allocation.xlsx
+++ b/RHNA/output/rhna_allocation.xlsx
@@ -1028,7 +1028,7 @@
         <v>32</v>
       </c>
       <c r="C8">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D8">
         <v>817</v>
@@ -1246,7 +1246,7 @@
         <v>44</v>
       </c>
       <c r="C20">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="D20">
         <v>847</v>
@@ -1300,7 +1300,7 @@
         <v>47</v>
       </c>
       <c r="C23">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D23">
         <v>126</v>
@@ -1309,7 +1309,7 @@
         <v>327</v>
       </c>
       <c r="F23">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1444,7 +1444,7 @@
         <v>55</v>
       </c>
       <c r="C31">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D31">
         <v>254</v>
@@ -1453,7 +1453,7 @@
         <v>657</v>
       </c>
       <c r="F31">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1635,7 +1635,7 @@
         <v>326</v>
       </c>
       <c r="F41">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1662,7 +1662,7 @@
         <v>67</v>
       </c>
       <c r="C43">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43">
         <v>16</v>
@@ -1761,7 +1761,7 @@
         <v>1323</v>
       </c>
       <c r="F48">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1826,7 +1826,7 @@
         <v>75</v>
       </c>
       <c r="C52">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D52">
         <v>26</v>
@@ -1835,7 +1835,7 @@
         <v>66</v>
       </c>
       <c r="F52">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2046,7 +2046,7 @@
         <v>86</v>
       </c>
       <c r="C64">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D64">
         <v>54</v>
@@ -2055,7 +2055,7 @@
         <v>141</v>
       </c>
       <c r="F64">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2172,7 +2172,7 @@
         <v>93</v>
       </c>
       <c r="C71">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D71">
         <v>573</v>
@@ -2235,7 +2235,7 @@
         <v>1863</v>
       </c>
       <c r="F74">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2444,7 +2444,7 @@
         <v>107</v>
       </c>
       <c r="C86">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D86">
         <v>1885</v>
@@ -2480,7 +2480,7 @@
         <v>109</v>
       </c>
       <c r="C88">
-        <v>8688</v>
+        <v>8689</v>
       </c>
       <c r="D88">
         <v>10711</v>
@@ -2608,7 +2608,7 @@
         <v>115</v>
       </c>
       <c r="C95">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D95">
         <v>508</v>
@@ -2880,7 +2880,7 @@
         <v>129</v>
       </c>
       <c r="C110">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D110">
         <v>108</v>
@@ -2889,7 +2889,7 @@
         <v>279</v>
       </c>
       <c r="F110">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed rounding for equity adjustment
Changed rounding in equity adjustment from np.ceil to np.round
</commit_message>
<xml_diff>
--- a/RHNA/output/rhna_allocation.xlsx
+++ b/RHNA/output/rhna_allocation.xlsx
@@ -929,7 +929,7 @@
         <v>2246</v>
       </c>
       <c r="F2">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1028,7 +1028,7 @@
         <v>32</v>
       </c>
       <c r="C8">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D8">
         <v>817</v>
@@ -1055,7 +1055,7 @@
         <v>1799</v>
       </c>
       <c r="F9">
-        <v>1316</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1091,7 +1091,7 @@
         <v>11533</v>
       </c>
       <c r="F11">
-        <v>6512</v>
+        <v>6511</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1163,7 +1163,7 @@
         <v>1976</v>
       </c>
       <c r="F15">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1246,7 +1246,7 @@
         <v>44</v>
       </c>
       <c r="C20">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D20">
         <v>847</v>
@@ -1300,7 +1300,7 @@
         <v>47</v>
       </c>
       <c r="C23">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D23">
         <v>126</v>
@@ -1309,7 +1309,7 @@
         <v>327</v>
       </c>
       <c r="F23">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1444,7 +1444,7 @@
         <v>55</v>
       </c>
       <c r="C31">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D31">
         <v>254</v>
@@ -1626,7 +1626,7 @@
         <v>65</v>
       </c>
       <c r="C41">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D41">
         <v>126</v>
@@ -1635,7 +1635,7 @@
         <v>326</v>
       </c>
       <c r="F41">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1662,7 +1662,7 @@
         <v>67</v>
       </c>
       <c r="C43">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D43">
         <v>16</v>
@@ -1752,7 +1752,7 @@
         <v>72</v>
       </c>
       <c r="C48">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D48">
         <v>512</v>
@@ -1835,7 +1835,7 @@
         <v>66</v>
       </c>
       <c r="F52">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1844,7 +1844,7 @@
         <v>76</v>
       </c>
       <c r="C53">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D53">
         <v>120</v>
@@ -1882,7 +1882,7 @@
         <v>22</v>
       </c>
       <c r="C55">
-        <v>12013</v>
+        <v>12014</v>
       </c>
       <c r="D55">
         <v>13717</v>
@@ -2172,7 +2172,7 @@
         <v>93</v>
       </c>
       <c r="C71">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D71">
         <v>573</v>
@@ -2417,7 +2417,7 @@
         <v>79</v>
       </c>
       <c r="F84">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2444,7 +2444,7 @@
         <v>107</v>
       </c>
       <c r="C86">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="D86">
         <v>1885</v>
@@ -2480,7 +2480,7 @@
         <v>109</v>
       </c>
       <c r="C88">
-        <v>8689</v>
+        <v>8687</v>
       </c>
       <c r="D88">
         <v>10711</v>
@@ -2489,7 +2489,7 @@
         <v>27714</v>
       </c>
       <c r="F88">
-        <v>15089</v>
+        <v>15088</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2561,7 +2561,7 @@
         <v>1312</v>
       </c>
       <c r="F92">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2608,7 +2608,7 @@
         <v>115</v>
       </c>
       <c r="C95">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D95">
         <v>508</v>
@@ -2808,7 +2808,7 @@
         <v>126</v>
       </c>
       <c r="C106">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D106">
         <v>771</v>
@@ -2880,7 +2880,7 @@
         <v>129</v>
       </c>
       <c r="C110">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D110">
         <v>108</v>

</xml_diff>